<commit_message>
Fix dots on graphs and soil n graphs for MCP910
</commit_message>
<xml_diff>
--- a/Tests/Validation/Barley/LeafSizeObserved.xlsx
+++ b/Tests/Validation/Barley/LeafSizeObserved.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\ApsimX\Prototypes\Barley\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Barley\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A54E1D-0B17-4EBB-A37A-E4F12C5E2F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeafSize" sheetId="1" r:id="rId1"/>
@@ -56,19 +57,19 @@
     <t>MCPD11_12CultOmakaSD3</t>
   </si>
   <si>
-    <t>SD</t>
-  </si>
-  <si>
     <t>MaxLeafSize.Script.LeafPosition</t>
   </si>
   <si>
     <t>MaxLeafSize.Script.MaxLeafSize</t>
   </si>
+  <si>
+    <t>SDx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,34 +381,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -421,7 +422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -435,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -449,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -463,7 +464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -477,7 +478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -491,7 +492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -505,7 +506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -519,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -533,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -547,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -561,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -575,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -589,7 +590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -603,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -617,7 +618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -631,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -645,7 +646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -659,7 +660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -673,7 +674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -687,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -701,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -715,7 +716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -727,7 +728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -741,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -755,7 +756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -769,7 +770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -783,7 +784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -797,7 +798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -811,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -825,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -839,7 +840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -853,7 +854,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -867,7 +868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -879,7 +880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -893,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -907,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -921,7 +922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -935,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -949,7 +950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -963,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -977,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -991,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1019,7 +1020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -1047,7 +1048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1089,7 +1090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>5</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>5</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>6</v>
       </c>
@@ -1227,7 +1228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -1255,7 +1256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -1353,7 +1354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -1409,7 +1410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -1521,7 +1522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -1591,7 +1592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -1671,7 +1672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>9</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -1713,7 +1714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -1797,7 +1798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>9</v>
       </c>

</xml_diff>